<commit_message>
changed plotting for NM, GRM
</commit_message>
<xml_diff>
--- a/01-lab/results/excel/golden_ratio_method.xlsx
+++ b/01-lab/results/excel/golden_ratio_method.xlsx
@@ -19,97 +19,11 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="27" uniqueCount="27">
-  <si>
-    <t xml:space="preserve">X_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 iteracija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 iteracija</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0E+00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -177,16 +91,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -314,304 +236,426 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
-    <col min="2" max="2" width="9.7109375" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
-    <col min="3" max="3" width="14.41" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="1" max="1" width="6.140625" style="1" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="5" max="6" width="14.41" style="1" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="2" max="2" width="6.140625" style="1" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="3" max="3" width="6.140625" style="1" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="4" max="4" width="6.140625" style="1" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1">
+      <c r="A1" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
         <v>3.819660112501051</v>
       </c>
-      <c r="B1" s="1">
+      <c r="C1" s="2">
         <v>6.180339887498949</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
+      <c r="D1" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
         <v>2.3606797749978967</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C2" s="3">
         <v>3.819660112501051</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>6.18033988749895</v>
-      </c>
+      <c r="D2" s="3">
+        <v>6.180339887498949</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
         <v>1.4589803375031543</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="3">
         <v>2.3606797749978967</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>3.81966011250105</v>
-      </c>
+      <c r="D3" s="3">
+        <v>3.819660112501051</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
         <v>0.90169943749474224</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="3">
         <v>1.4589803375031543</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>2.3606797749979</v>
-      </c>
+      <c r="D4" s="3">
+        <v>2.3606797749978967</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3">
         <v>0.55728090000841191</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C5" s="3">
         <v>0.90169943749474224</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>1.45898033750315</v>
-      </c>
+      <c r="D5" s="3">
+        <v>1.4589803375031543</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
+        <v>0.55728090000841191</v>
+      </c>
+      <c r="B6" s="3">
         <v>0.90169943749474224</v>
       </c>
-      <c r="B6" s="2">
+      <c r="C6" s="3">
         <v>1.114561800016824</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>0.901699437494742</v>
-      </c>
+      <c r="D6" s="3">
+        <v>1.4589803375031543</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
+        <v>0.55728090000841191</v>
+      </c>
+      <c r="B7" s="3">
         <v>0.77014326253049381</v>
       </c>
-      <c r="B7" s="2">
+      <c r="C7" s="3">
         <v>0.90169943749474224</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>1.11456180001682</v>
-      </c>
+      <c r="D7" s="3">
+        <v>1.114561800016824</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
+        <v>0.77014326253049381</v>
+      </c>
+      <c r="B8" s="3">
         <v>0.90169943749474224</v>
       </c>
-      <c r="B8" s="2">
+      <c r="C8" s="3">
         <v>0.98300562505257572</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>0.901699437494742</v>
-      </c>
+      <c r="D8" s="3">
+        <v>1.114561800016824</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
+        <v>0.90169943749474224</v>
+      </c>
+      <c r="B9" s="3">
         <v>0.98300562505257572</v>
       </c>
-      <c r="B9" s="2">
+      <c r="C9" s="3">
         <v>1.0332556124589907</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>0.983005625052576</v>
-      </c>
+      <c r="D9" s="3">
+        <v>1.114561800016824</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
+        <v>0.90169943749474224</v>
+      </c>
+      <c r="B10" s="3">
         <v>0.95194942490115719</v>
       </c>
-      <c r="B10" s="2">
+      <c r="C10" s="3">
         <v>0.98300562505257572</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>1.03325561245899</v>
-      </c>
+      <c r="D10" s="3">
+        <v>1.0332556124589907</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
+        <v>0.95194942490115719</v>
+      </c>
+      <c r="B11" s="3">
         <v>0.98300562505257572</v>
       </c>
-      <c r="B11" s="2">
-        <v>1.0021994123075721</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>0.983005625052576</v>
-      </c>
+      <c r="C11" s="3">
+        <v>1.0021994123075721</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.0332556124589907</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1">
-        <v>1.0021994123075721</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="A12" s="2">
+        <v>0.98300562505257572</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.0021994123075721</v>
+      </c>
+      <c r="C12" s="3">
         <v>1.0140618252039943</v>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>1.00219941230757</v>
-      </c>
+      <c r="D12" s="3">
+        <v>1.0332556124589907</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
+        <v>0.98300562505257572</v>
+      </c>
+      <c r="B13" s="3">
         <v>0.99486803794899803</v>
       </c>
-      <c r="B13" s="2">
-        <v>1.0021994123075721</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>1.01406182520399</v>
-      </c>
+      <c r="C13" s="3">
+        <v>1.0021994123075721</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.0140618252039943</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1">
-        <v>1.0021994123075721</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="A14" s="2">
+        <v>0.99486803794899803</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.0021994123075721</v>
+      </c>
+      <c r="C14" s="3">
         <v>1.0067304508454202</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>1.00219941230757</v>
-      </c>
+      <c r="D14" s="3">
+        <v>1.0140618252039943</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
+        <v>0.99486803794899803</v>
+      </c>
+      <c r="B15" s="3">
         <v>0.99939907648684623</v>
       </c>
-      <c r="B15" s="2">
-        <v>1.0021994123075721</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>1.00673045084542</v>
-      </c>
+      <c r="C15" s="3">
+        <v>1.0021994123075721</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1.0067304508454202</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
+        <v>0.99486803794899803</v>
+      </c>
+      <c r="B16" s="3">
         <v>0.99766837376972384</v>
       </c>
-      <c r="B16" s="2">
+      <c r="C16" s="3">
         <v>0.99939907648684623</v>
       </c>
-      <c r="C16" s="2" t="n">
-        <v>1.00219941230757</v>
-      </c>
+      <c r="D16" s="3">
+        <v>1.0021994123075721</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
+        <v>0.99766837376972384</v>
+      </c>
+      <c r="B17" s="3">
         <v>0.99939907648684623</v>
       </c>
-      <c r="B17" s="2">
+      <c r="C17" s="3">
         <v>1.0004687095904496</v>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>0.999399076486846</v>
-      </c>
+      <c r="D17" s="3">
+        <v>1.0021994123075721</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
+        <v>0.99939907648684623</v>
+      </c>
+      <c r="B18" s="3">
         <v>1.0004687095904496</v>
       </c>
-      <c r="B18" s="2">
+      <c r="C18" s="3">
         <v>1.0011297792039686</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>1.00046870959045</v>
-      </c>
+      <c r="D18" s="3">
+        <v>1.0021994123075721</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
+        <v>0.99939907648684623</v>
+      </c>
+      <c r="B19" s="3">
         <v>1.0000601461003651</v>
       </c>
-      <c r="B19" s="2">
+      <c r="C19" s="3">
         <v>1.0004687095904496</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>1.00112977920397</v>
-      </c>
+      <c r="D19" s="3">
+        <v>1.0011297792039686</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
+        <v>0.99939907648684623</v>
+      </c>
+      <c r="B20" s="3">
         <v>0.99980763997693067</v>
       </c>
-      <c r="B20" s="2">
+      <c r="C20" s="3">
         <v>1.0000601461003651</v>
       </c>
-      <c r="C20" s="2" t="n">
-        <v>1.00046870959045</v>
-      </c>
+      <c r="D20" s="3">
+        <v>1.0004687095904496</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
+        <v>0.99980763997693067</v>
+      </c>
+      <c r="B21" s="3">
         <v>1.0000601461003651</v>
       </c>
-      <c r="B21" s="2">
+      <c r="C21" s="3">
         <v>1.0002162034670152</v>
       </c>
-      <c r="C21" s="2" t="n">
-        <v>1.00006014610037</v>
-      </c>
+      <c r="D21" s="3">
+        <v>1.0004687095904496</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
+        <v>0.99980763997693067</v>
+      </c>
+      <c r="B22" s="3">
         <v>0.9999636973435807</v>
       </c>
-      <c r="B22" s="2">
+      <c r="C22" s="3">
         <v>1.0000601461003651</v>
       </c>
-      <c r="C22" s="2" t="n">
-        <v>1.00021620346702</v>
-      </c>
+      <c r="D22" s="3">
+        <v>1.0002162034670152</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
+        <v>0.99980763997693067</v>
+      </c>
+      <c r="B23" s="3">
         <v>0.99990408873371517</v>
       </c>
-      <c r="B23" s="2">
+      <c r="C23" s="3">
         <v>0.9999636973435807</v>
       </c>
-      <c r="C23" s="2" t="n">
-        <v>1.00006014610037</v>
-      </c>
+      <c r="D23" s="3">
+        <v>1.0000601461003651</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
+        <v>0.99990408873371517</v>
+      </c>
+      <c r="B24" s="3">
         <v>0.9999636973435807</v>
       </c>
-      <c r="B24" s="2">
+      <c r="C24" s="3">
         <v>1.0000005374904997</v>
       </c>
-      <c r="C24" s="2" t="n">
-        <v>0.999963697343581</v>
-      </c>
+      <c r="D24" s="3">
+        <v>1.0000601461003651</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
+        <v>0.9999636973435807</v>
+      </c>
+      <c r="B25" s="3">
         <v>1.0000005374904997</v>
       </c>
-      <c r="B25" s="2">
+      <c r="C25" s="3">
         <v>1.000023305953446</v>
       </c>
-      <c r="C25" s="2" t="n">
-        <v>1.0000005374905</v>
-      </c>
+      <c r="D25" s="3">
+        <v>1.0000601461003651</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="2" t="n">
-        <v>1.0000005374905</v>
-      </c>
-      <c r="C26" s="2" t="n">
-        <v>1.00002330595345</v>
-      </c>
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="false" verticalCentered="false" headings="false" gridLines="false" gridLinesSet="true"/>

</xml_diff>